<commit_message>
Begin to introduce support for a few named colors
</commit_message>
<xml_diff>
--- a/data/Borders.xlsx
+++ b/data/Borders.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee85442dac9ca7a7/Documents/Julia/XLSX/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee85442dac9ca7a7/Documents/Julia/XLSX/XLSX.jl/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{EA0591A3-802F-4C6A-8185-454648B76ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F165503-665C-413C-9EC7-FDDBBBEABE3E}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{EA0591A3-802F-4C6A-8185-454648B76ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67B71AF7-7547-4886-85A4-DD300565427F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{043A91C4-BD91-4085-AEB2-3DA5799D0A9E}"/>
   </bookViews>
@@ -228,6 +228,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF0000"/>
+      <color rgb="FFFF0003"/>
+      <color rgb="FFFF0004"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -237,6 +244,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -559,7 +570,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>